<commit_message>
Updated DocType codelist and XSD
</commit_message>
<xml_diff>
--- a/publication/v9.1/Peppol Code Lists - Document types v9.1.xlsx
+++ b/publication/v9.1/Peppol Code Lists - Document types v9.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philip/dev/git-peppol/edec-codelists/work-in-progress/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BE87DE-0293-4139-BDC9-0560BB0DE064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4A8EB2-BD4C-6E4D-B97E-260DA47977C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25410" yWindow="135" windowWidth="25560" windowHeight="20745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
@@ -2745,7 +2745,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2887,6 +2887,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3304,30 +3307,30 @@
   <dimension ref="A1:N303"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A292" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A304" sqref="A304"/>
+      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A230" sqref="A230"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="6" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="23"/>
-    <col min="12" max="12" width="19.140625" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.140625" style="23" customWidth="1"/>
-    <col min="14" max="14" width="84.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="5"/>
+    <col min="7" max="7" width="15.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" style="5" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="23"/>
+    <col min="12" max="12" width="19.1640625" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" style="23" customWidth="1"/>
+    <col min="14" max="14" width="84.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.5" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>117</v>
       </c>
@@ -3371,7 +3374,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>7</v>
       </c>
@@ -3411,7 +3414,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
         <v>8</v>
       </c>
@@ -3451,7 +3454,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
         <v>9</v>
       </c>
@@ -3491,7 +3494,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>96</v>
       </c>
@@ -3531,7 +3534,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>98</v>
       </c>
@@ -3571,7 +3574,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>98</v>
       </c>
@@ -3611,7 +3614,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>36</v>
       </c>
@@ -3651,7 +3654,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
         <v>28</v>
       </c>
@@ -3691,7 +3694,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="31" t="s">
         <v>336</v>
       </c>
@@ -3734,7 +3737,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="31" t="s">
         <v>29</v>
       </c>
@@ -3774,7 +3777,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
         <v>25</v>
       </c>
@@ -3814,7 +3817,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
         <v>26</v>
       </c>
@@ -3854,7 +3857,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
         <v>97</v>
       </c>
@@ -3894,7 +3897,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="31" t="s">
         <v>752</v>
       </c>
@@ -3934,7 +3937,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="31" t="s">
         <v>97</v>
       </c>
@@ -3974,7 +3977,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="31" t="s">
         <v>89</v>
       </c>
@@ -4014,7 +4017,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="31" t="s">
         <v>753</v>
       </c>
@@ -4054,7 +4057,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
         <v>93</v>
       </c>
@@ -4094,7 +4097,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A20" s="36" t="s">
         <v>94</v>
       </c>
@@ -4134,7 +4137,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
         <v>94</v>
       </c>
@@ -4174,7 +4177,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
         <v>95</v>
       </c>
@@ -4214,7 +4217,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
         <v>754</v>
       </c>
@@ -4254,7 +4257,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="36" t="s">
         <v>95</v>
       </c>
@@ -4294,7 +4297,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="36" t="s">
         <v>34</v>
       </c>
@@ -4332,7 +4335,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>35</v>
       </c>
@@ -4365,7 +4368,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="36" t="s">
         <v>91</v>
       </c>
@@ -4405,7 +4408,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="36" t="s">
         <v>333</v>
       </c>
@@ -4448,7 +4451,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A29" s="36" t="s">
         <v>92</v>
       </c>
@@ -4488,7 +4491,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="36" t="s">
         <v>39</v>
       </c>
@@ -4528,7 +4531,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="36" t="s">
         <v>40</v>
       </c>
@@ -4568,7 +4571,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>450</v>
       </c>
@@ -4607,7 +4610,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>757</v>
       </c>
@@ -4646,7 +4649,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>90</v>
       </c>
@@ -4679,7 +4682,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
         <v>330</v>
       </c>
@@ -4720,7 +4723,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>118</v>
       </c>
@@ -4756,7 +4759,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>451</v>
       </c>
@@ -4792,7 +4795,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="36" t="s">
         <v>466</v>
       </c>
@@ -4835,7 +4838,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="36" t="s">
         <v>465</v>
       </c>
@@ -4878,7 +4881,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="36" t="s">
         <v>464</v>
       </c>
@@ -4921,7 +4924,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="41" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A41" s="36" t="s">
         <v>463</v>
       </c>
@@ -4964,7 +4967,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" s="36" t="s">
         <v>462</v>
       </c>
@@ -5007,7 +5010,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="36" t="s">
         <v>461</v>
       </c>
@@ -5050,7 +5053,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="44" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
         <v>99</v>
       </c>
@@ -5093,7 +5096,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
         <v>755</v>
       </c>
@@ -5136,7 +5139,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
         <v>100</v>
       </c>
@@ -5179,7 +5182,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
         <v>61</v>
       </c>
@@ -5215,7 +5218,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
         <v>62</v>
       </c>
@@ -5251,7 +5254,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
         <v>63</v>
       </c>
@@ -5287,7 +5290,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
         <v>64</v>
       </c>
@@ -5323,7 +5326,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="51" spans="1:14" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="36" t="s">
         <v>440</v>
       </c>
@@ -5363,7 +5366,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
         <v>441</v>
       </c>
@@ -5399,7 +5402,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
         <v>442</v>
       </c>
@@ -5435,7 +5438,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
         <v>443</v>
       </c>
@@ -5474,7 +5477,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
         <v>444</v>
       </c>
@@ -5513,7 +5516,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
         <v>446</v>
       </c>
@@ -5549,7 +5552,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
         <v>445</v>
       </c>
@@ -5585,7 +5588,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
         <v>447</v>
       </c>
@@ -5621,7 +5624,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
         <v>448</v>
       </c>
@@ -5657,7 +5660,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
         <v>449</v>
       </c>
@@ -5693,7 +5696,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
         <v>79</v>
       </c>
@@ -5726,7 +5729,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
         <v>756</v>
       </c>
@@ -5759,7 +5762,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
         <v>452</v>
       </c>
@@ -5795,7 +5798,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="36" t="s">
         <v>331</v>
       </c>
@@ -5838,7 +5841,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
         <v>453</v>
       </c>
@@ -5877,7 +5880,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="66" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="s">
         <v>84</v>
       </c>
@@ -5920,7 +5923,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="67" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
         <v>758</v>
       </c>
@@ -5963,7 +5966,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A68" s="15" t="s">
         <v>85</v>
       </c>
@@ -6006,7 +6009,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
         <v>101</v>
       </c>
@@ -6042,7 +6045,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
         <v>102</v>
       </c>
@@ -6078,7 +6081,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
         <v>106</v>
       </c>
@@ -6114,7 +6117,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>454</v>
       </c>
@@ -6153,7 +6156,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>759</v>
       </c>
@@ -6192,7 +6195,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
         <v>112</v>
       </c>
@@ -6228,7 +6231,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
         <v>760</v>
       </c>
@@ -6264,7 +6267,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="76" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
         <v>153</v>
       </c>
@@ -6307,7 +6310,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="77" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A77" s="15" t="s">
         <v>156</v>
       </c>
@@ -6350,7 +6353,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="78" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
         <v>158</v>
       </c>
@@ -6393,7 +6396,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="79" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A79" s="15" t="s">
         <v>761</v>
       </c>
@@ -6436,7 +6439,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="80" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
         <v>159</v>
       </c>
@@ -6479,7 +6482,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
         <v>162</v>
       </c>
@@ -6515,7 +6518,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
         <v>763</v>
       </c>
@@ -6551,7 +6554,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="83" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="15" t="s">
         <v>228</v>
       </c>
@@ -6594,7 +6597,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
         <v>163</v>
       </c>
@@ -6630,7 +6633,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="85" spans="1:14" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" s="15" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A85" s="15" t="s">
         <v>166</v>
       </c>
@@ -6673,7 +6676,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="86" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="s">
         <v>762</v>
       </c>
@@ -6716,7 +6719,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="87" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="15" t="s">
         <v>167</v>
       </c>
@@ -6759,7 +6762,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
         <v>172</v>
       </c>
@@ -6795,7 +6798,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="89" spans="1:14" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="36" t="s">
         <v>219</v>
       </c>
@@ -6836,7 +6839,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="90" spans="1:14" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="36" t="s">
         <v>220</v>
       </c>
@@ -6877,7 +6880,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="91" spans="1:14" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" s="36" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="36" t="s">
         <v>221</v>
       </c>
@@ -6918,7 +6921,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="92" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A92" s="36" t="s">
         <v>222</v>
       </c>
@@ -6959,7 +6962,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
         <v>184</v>
       </c>
@@ -6995,7 +6998,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>765</v>
       </c>
@@ -7031,7 +7034,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>185</v>
       </c>
@@ -7067,7 +7070,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>190</v>
       </c>
@@ -7103,7 +7106,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>764</v>
       </c>
@@ -7139,7 +7142,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="98" spans="1:14" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" s="15" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A98" s="15" t="s">
         <v>232</v>
       </c>
@@ -7182,7 +7185,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>191</v>
       </c>
@@ -7218,7 +7221,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
         <v>208</v>
       </c>
@@ -7254,7 +7257,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>209</v>
       </c>
@@ -7290,7 +7293,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="8" t="s">
         <v>210</v>
       </c>
@@ -7326,7 +7329,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="103" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="15" t="s">
         <v>218</v>
       </c>
@@ -7367,7 +7370,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
         <v>173</v>
       </c>
@@ -7403,7 +7406,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
         <v>174</v>
       </c>
@@ -7439,7 +7442,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
         <v>175</v>
       </c>
@@ -7475,7 +7478,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>176</v>
       </c>
@@ -7511,7 +7514,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>238</v>
       </c>
@@ -7547,7 +7550,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>239</v>
       </c>
@@ -7583,7 +7586,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>240</v>
       </c>
@@ -7619,7 +7622,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>241</v>
       </c>
@@ -7655,7 +7658,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>242</v>
       </c>
@@ -7691,7 +7694,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>243</v>
       </c>
@@ -7727,7 +7730,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>244</v>
       </c>
@@ -7763,7 +7766,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>245</v>
       </c>
@@ -7799,7 +7802,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>246</v>
       </c>
@@ -7835,7 +7838,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>247</v>
       </c>
@@ -7871,7 +7874,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>248</v>
       </c>
@@ -7907,7 +7910,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>249</v>
       </c>
@@ -7943,7 +7946,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>250</v>
       </c>
@@ -7979,7 +7982,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>251</v>
       </c>
@@ -8015,7 +8018,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>252</v>
       </c>
@@ -8051,7 +8054,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>253</v>
       </c>
@@ -8087,7 +8090,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>254</v>
       </c>
@@ -8123,7 +8126,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>255</v>
       </c>
@@ -8159,7 +8162,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>256</v>
       </c>
@@ -8195,7 +8198,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>257</v>
       </c>
@@ -8231,7 +8234,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>258</v>
       </c>
@@ -8267,7 +8270,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>259</v>
       </c>
@@ -8303,7 +8306,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="5" t="s">
         <v>455</v>
       </c>
@@ -8341,7 +8344,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
         <v>456</v>
       </c>
@@ -8379,7 +8382,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A132" s="5" t="s">
         <v>457</v>
       </c>
@@ -8417,7 +8420,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="5" t="s">
         <v>458</v>
       </c>
@@ -8455,7 +8458,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A134" s="5" t="s">
         <v>292</v>
       </c>
@@ -8490,7 +8493,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A135" s="5" t="s">
         <v>293</v>
       </c>
@@ -8525,7 +8528,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
         <v>294</v>
       </c>
@@ -8560,7 +8563,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A137" s="5" t="s">
         <v>295</v>
       </c>
@@ -8595,7 +8598,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A138" s="5" t="s">
         <v>296</v>
       </c>
@@ -8630,7 +8633,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
         <v>297</v>
       </c>
@@ -8665,7 +8668,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="5" t="s">
         <v>298</v>
       </c>
@@ -8700,7 +8703,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A141" s="5" t="s">
         <v>299</v>
       </c>
@@ -8735,7 +8738,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
         <v>300</v>
       </c>
@@ -8770,7 +8773,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
         <v>301</v>
       </c>
@@ -8805,7 +8808,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A144" s="5" t="s">
         <v>302</v>
       </c>
@@ -8840,7 +8843,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="5" t="s">
         <v>303</v>
       </c>
@@ -8875,7 +8878,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A146" s="5" t="s">
         <v>304</v>
       </c>
@@ -8910,7 +8913,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A147" s="5" t="s">
         <v>305</v>
       </c>
@@ -8945,7 +8948,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="5" t="s">
         <v>337</v>
       </c>
@@ -8980,7 +8983,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A149" s="5" t="s">
         <v>766</v>
       </c>
@@ -9015,7 +9018,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A150" s="5" t="s">
         <v>338</v>
       </c>
@@ -9050,7 +9053,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A151" s="5" t="s">
         <v>343</v>
       </c>
@@ -9085,7 +9088,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A152" s="5" t="s">
         <v>767</v>
       </c>
@@ -9120,7 +9123,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A153" s="5" t="s">
         <v>344</v>
       </c>
@@ -9155,7 +9158,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="154" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
         <v>360</v>
       </c>
@@ -9190,7 +9193,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A155" s="5" t="s">
         <v>361</v>
       </c>
@@ -9225,7 +9228,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A156" s="5" t="s">
         <v>362</v>
       </c>
@@ -9260,7 +9263,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="157" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A157" s="5" t="s">
         <v>374</v>
       </c>
@@ -9298,7 +9301,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A158" s="5" t="s">
         <v>375</v>
       </c>
@@ -9336,7 +9339,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A159" s="5" t="s">
         <v>376</v>
       </c>
@@ -9374,7 +9377,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A160" s="5" t="s">
         <v>377</v>
       </c>
@@ -9412,7 +9415,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A161" s="5" t="s">
         <v>378</v>
       </c>
@@ -9450,7 +9453,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="5" t="s">
         <v>379</v>
       </c>
@@ -9488,7 +9491,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="5" t="s">
         <v>380</v>
       </c>
@@ -9526,7 +9529,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="5" t="s">
         <v>381</v>
       </c>
@@ -9564,7 +9567,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="5" t="s">
         <v>382</v>
       </c>
@@ -9602,7 +9605,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="5" t="s">
         <v>383</v>
       </c>
@@ -9640,7 +9643,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="5" t="s">
         <v>384</v>
       </c>
@@ -9678,7 +9681,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="5" t="s">
         <v>385</v>
       </c>
@@ -9716,7 +9719,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="5" t="s">
         <v>386</v>
       </c>
@@ -9754,7 +9757,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="5" t="s">
         <v>387</v>
       </c>
@@ -9792,7 +9795,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" s="5" t="s">
         <v>390</v>
       </c>
@@ -9830,7 +9833,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="5" t="s">
         <v>389</v>
       </c>
@@ -9868,7 +9871,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="173" spans="1:14" s="36" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" s="36" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A173" s="36" t="s">
         <v>542</v>
       </c>
@@ -9910,7 +9913,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="5" t="s">
         <v>388</v>
       </c>
@@ -9948,7 +9951,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="5" t="s">
         <v>411</v>
       </c>
@@ -9983,7 +9986,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="5" t="s">
         <v>768</v>
       </c>
@@ -10018,7 +10021,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A177" s="5" t="s">
         <v>412</v>
       </c>
@@ -10053,7 +10056,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="178" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="5" t="s">
         <v>413</v>
       </c>
@@ -10088,7 +10091,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="179" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="5" t="s">
         <v>769</v>
       </c>
@@ -10123,7 +10126,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A180" s="5" t="s">
         <v>414</v>
       </c>
@@ -10158,7 +10161,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="181" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="44" t="s">
         <v>459</v>
       </c>
@@ -10200,7 +10203,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="182" spans="1:14" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="44" t="s">
         <v>460</v>
       </c>
@@ -10242,7 +10245,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="183" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A183" s="5" t="s">
         <v>552</v>
       </c>
@@ -10280,7 +10283,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="184" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="5" t="s">
         <v>553</v>
       </c>
@@ -10318,7 +10321,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="185" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A185" s="5" t="s">
         <v>554</v>
       </c>
@@ -10356,7 +10359,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="186" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A186" s="5" t="s">
         <v>435</v>
       </c>
@@ -10391,7 +10394,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="187" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A187" s="5" t="s">
         <v>467</v>
       </c>
@@ -10426,7 +10429,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="188" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A188" s="44" t="s">
         <v>470</v>
       </c>
@@ -10471,7 +10474,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="189" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A189" s="5" t="s">
         <v>478</v>
       </c>
@@ -10509,7 +10512,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="190" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A190" s="5" t="s">
         <v>479</v>
       </c>
@@ -10547,7 +10550,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="191" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A191" s="5" t="s">
         <v>480</v>
       </c>
@@ -10585,7 +10588,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="192" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A192" s="5" t="s">
         <v>494</v>
       </c>
@@ -10620,7 +10623,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="193" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="5" t="s">
         <v>771</v>
       </c>
@@ -10655,7 +10658,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="194" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A194" s="5" t="s">
         <v>495</v>
       </c>
@@ -10690,7 +10693,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="195" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A195" s="5" t="s">
         <v>496</v>
       </c>
@@ -10725,7 +10728,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="196" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A196" s="5" t="s">
         <v>772</v>
       </c>
@@ -10760,7 +10763,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="197" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A197" s="5" t="s">
         <v>497</v>
       </c>
@@ -10795,7 +10798,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="198" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:14" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A198" s="44" t="s">
         <v>504</v>
       </c>
@@ -10840,7 +10843,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="199" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A199" s="5" t="s">
         <v>508</v>
       </c>
@@ -10879,7 +10882,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="200" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A200" s="5" t="s">
         <v>509</v>
       </c>
@@ -10918,7 +10921,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="201" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A201" s="5" t="s">
         <v>513</v>
       </c>
@@ -10957,7 +10960,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="202" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A202" s="5" t="s">
         <v>514</v>
       </c>
@@ -10996,7 +10999,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="203" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A203" s="5" t="s">
         <v>518</v>
       </c>
@@ -11034,7 +11037,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="204" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A204" s="5" t="s">
         <v>519</v>
       </c>
@@ -11072,7 +11075,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A205" s="5" t="s">
         <v>523</v>
       </c>
@@ -11110,7 +11113,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="206" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A206" s="5" t="s">
         <v>524</v>
       </c>
@@ -11148,7 +11151,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A207" s="5" t="s">
         <v>529</v>
       </c>
@@ -11186,7 +11189,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="208" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A208" s="5" t="s">
         <v>528</v>
       </c>
@@ -11224,7 +11227,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="209" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A209" s="5" t="s">
         <v>533</v>
       </c>
@@ -11262,7 +11265,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="210" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A210" s="5" t="s">
         <v>534</v>
       </c>
@@ -11300,7 +11303,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="211" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A211" s="5" t="s">
         <v>544</v>
       </c>
@@ -11338,7 +11341,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="212" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A212" s="5" t="s">
         <v>546</v>
       </c>
@@ -11376,7 +11379,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="213" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A213" s="5" t="s">
         <v>547</v>
       </c>
@@ -11414,7 +11417,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="214" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A214" s="5" t="s">
         <v>556</v>
       </c>
@@ -11452,7 +11455,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="215" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A215" s="5" t="s">
         <v>557</v>
       </c>
@@ -11490,7 +11493,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="216" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A216" s="5" t="s">
         <v>558</v>
       </c>
@@ -11528,7 +11531,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="217" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A217" s="5" t="s">
         <v>559</v>
       </c>
@@ -11566,7 +11569,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="218" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A218" s="5" t="s">
         <v>560</v>
       </c>
@@ -11604,7 +11607,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="219" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A219" s="5" t="s">
         <v>561</v>
       </c>
@@ -11642,7 +11645,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A220" s="5" t="s">
         <v>576</v>
       </c>
@@ -11677,7 +11680,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="221" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A221" s="5" t="s">
         <v>581</v>
       </c>
@@ -11712,7 +11715,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="222" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A222" s="5" t="s">
         <v>582</v>
       </c>
@@ -11747,7 +11750,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A223" s="5" t="s">
         <v>592</v>
       </c>
@@ -11785,7 +11788,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A224" s="5" t="s">
         <v>770</v>
       </c>
@@ -11823,7 +11826,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="225" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:14" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A225" s="44" t="s">
         <v>595</v>
       </c>
@@ -11867,7 +11870,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>595</v>
       </c>
@@ -11905,7 +11908,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>504</v>
       </c>
@@ -11943,7 +11946,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="228" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" s="15" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A228" s="44" t="s">
         <v>596</v>
       </c>
@@ -11987,7 +11990,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="229" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>596</v>
       </c>
@@ -12025,183 +12028,183 @@
         <v>591</v>
       </c>
     </row>
-    <row r="230" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A230" s="36" t="s">
+    <row r="230" spans="1:14" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A230" s="15" t="s">
         <v>598</v>
       </c>
-      <c r="B230" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="C230" s="36" t="s">
+      <c r="B230" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C230" s="15" t="s">
         <v>599</v>
       </c>
-      <c r="D230" s="32" t="s">
+      <c r="D230" s="29" t="s">
         <v>569</v>
       </c>
-      <c r="E230" s="33" t="s">
-        <v>351</v>
-      </c>
-      <c r="F230" s="41" t="s">
+      <c r="E230" s="24" t="s">
+        <v>482</v>
+      </c>
+      <c r="F230" s="52" t="s">
         <v>740</v>
       </c>
-      <c r="G230" s="35">
+      <c r="G230" s="18">
         <v>45717</v>
       </c>
-      <c r="H230" s="36" t="s">
+      <c r="H230" s="15" t="s">
         <v>751</v>
       </c>
-      <c r="I230" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="J230" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="K230" s="33">
+      <c r="I230" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J230" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K230" s="24">
         <v>3</v>
       </c>
-      <c r="L230" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="M230" s="33" t="s">
+      <c r="L230" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="M230" s="24" t="s">
         <v>693</v>
       </c>
-      <c r="N230" s="36" t="s">
+      <c r="N230" s="15" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="231" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A231" s="36" t="s">
+    <row r="231" spans="1:14" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A231" s="15" t="s">
         <v>600</v>
       </c>
-      <c r="B231" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="C231" s="36" t="s">
+      <c r="B231" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C231" s="15" t="s">
         <v>601</v>
       </c>
-      <c r="D231" s="32" t="s">
+      <c r="D231" s="29" t="s">
         <v>569</v>
       </c>
-      <c r="E231" s="33" t="s">
-        <v>351</v>
-      </c>
-      <c r="F231" s="41" t="s">
+      <c r="E231" s="24" t="s">
+        <v>482</v>
+      </c>
+      <c r="F231" s="52" t="s">
         <v>740</v>
       </c>
-      <c r="G231" s="35">
+      <c r="G231" s="18">
         <v>45717</v>
       </c>
-      <c r="H231" s="36" t="s">
+      <c r="H231" s="15" t="s">
         <v>751</v>
       </c>
-      <c r="I231" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="J231" s="36" t="b">
-        <v>1</v>
-      </c>
-      <c r="K231" s="33">
+      <c r="I231" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J231" s="15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K231" s="24">
         <v>3</v>
       </c>
-      <c r="L231" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="M231" s="33" t="s">
+      <c r="L231" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="M231" s="24" t="s">
         <v>694</v>
       </c>
-      <c r="N231" s="36" t="s">
+      <c r="N231" s="15" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="232" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A232" s="36" t="s">
+    <row r="232" spans="1:14" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A232" s="15" t="s">
         <v>602</v>
       </c>
-      <c r="B232" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="C232" s="36" t="s">
+      <c r="B232" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C232" s="15" t="s">
         <v>603</v>
       </c>
-      <c r="D232" s="32" t="s">
+      <c r="D232" s="29" t="s">
         <v>569</v>
       </c>
-      <c r="E232" s="33" t="s">
-        <v>351</v>
-      </c>
-      <c r="F232" s="41" t="s">
+      <c r="E232" s="24" t="s">
+        <v>482</v>
+      </c>
+      <c r="F232" s="52" t="s">
         <v>740</v>
       </c>
-      <c r="G232" s="35">
+      <c r="G232" s="18">
         <v>45717</v>
       </c>
-      <c r="H232" s="36" t="s">
+      <c r="H232" s="15" t="s">
         <v>751</v>
       </c>
-      <c r="I232" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="J232" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="K232" s="33">
+      <c r="I232" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J232" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K232" s="24">
         <v>3</v>
       </c>
-      <c r="L232" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="M232" s="33" t="s">
+      <c r="L232" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="M232" s="24" t="s">
         <v>693</v>
       </c>
-      <c r="N232" s="36" t="s">
+      <c r="N232" s="15" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="233" spans="1:14" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A233" s="36" t="s">
+    <row r="233" spans="1:14" s="15" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A233" s="15" t="s">
         <v>604</v>
       </c>
-      <c r="B233" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="C233" s="36" t="s">
+      <c r="B233" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C233" s="15" t="s">
         <v>605</v>
       </c>
-      <c r="D233" s="32" t="s">
+      <c r="D233" s="29" t="s">
         <v>569</v>
       </c>
-      <c r="E233" s="33" t="s">
-        <v>351</v>
-      </c>
-      <c r="F233" s="41" t="s">
+      <c r="E233" s="24" t="s">
+        <v>482</v>
+      </c>
+      <c r="F233" s="52" t="s">
         <v>740</v>
       </c>
-      <c r="G233" s="35">
+      <c r="G233" s="18">
         <v>45717</v>
       </c>
-      <c r="H233" s="36" t="s">
+      <c r="H233" s="15" t="s">
         <v>751</v>
       </c>
-      <c r="I233" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="J233" s="36" t="b">
-        <v>0</v>
-      </c>
-      <c r="K233" s="33">
+      <c r="I233" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J233" s="15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K233" s="24">
         <v>3</v>
       </c>
-      <c r="L233" s="33" t="s">
-        <v>111</v>
-      </c>
-      <c r="M233" s="33" t="s">
+      <c r="L233" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="M233" s="24" t="s">
         <v>694</v>
       </c>
-      <c r="N233" s="36" t="s">
+      <c r="N233" s="15" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A234" s="5" t="s">
         <v>598</v>
       </c>
@@ -12239,7 +12242,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="235" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A235" s="5" t="s">
         <v>600</v>
       </c>
@@ -12277,7 +12280,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="236" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A236" s="5" t="s">
         <v>602</v>
       </c>
@@ -12315,7 +12318,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="237" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A237" s="5" t="s">
         <v>604</v>
       </c>
@@ -12353,7 +12356,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="238" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A238" s="5" t="s">
         <v>609</v>
       </c>
@@ -12388,7 +12391,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="239" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A239" s="5" t="s">
         <v>773</v>
       </c>
@@ -12423,7 +12426,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="240" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A240" s="5" t="s">
         <v>610</v>
       </c>
@@ -12458,7 +12461,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="241" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A241" s="5" t="s">
         <v>611</v>
       </c>
@@ -12493,7 +12496,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="242" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A242" s="5" t="s">
         <v>774</v>
       </c>
@@ -12528,7 +12531,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="243" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A243" s="5" t="s">
         <v>612</v>
       </c>
@@ -12563,7 +12566,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="244" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A244" s="5" t="s">
         <v>622</v>
       </c>
@@ -12601,7 +12604,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="245" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A245" s="5" t="s">
         <v>621</v>
       </c>
@@ -12639,7 +12642,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="246" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>633</v>
       </c>
@@ -12677,7 +12680,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="247" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>634</v>
       </c>
@@ -12715,7 +12718,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="248" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>635</v>
       </c>
@@ -12753,7 +12756,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="249" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>636</v>
       </c>
@@ -12791,7 +12794,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="250" spans="1:14" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:14" s="45" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A250" s="48" t="s">
         <v>633</v>
       </c>
@@ -12835,7 +12838,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="251" spans="1:14" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:14" s="45" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A251" s="48" t="s">
         <v>634</v>
       </c>
@@ -12879,7 +12882,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="252" spans="1:14" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:14" s="45" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A252" s="48" t="s">
         <v>635</v>
       </c>
@@ -12923,7 +12926,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="253" spans="1:14" s="45" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:14" s="45" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A253" s="48" t="s">
         <v>636</v>
       </c>
@@ -12967,7 +12970,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="254" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A254" s="5" t="s">
         <v>643</v>
       </c>
@@ -13002,7 +13005,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="255" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A255" s="5" t="s">
         <v>648</v>
       </c>
@@ -13037,7 +13040,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="256" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A256" s="5" t="s">
         <v>649</v>
       </c>
@@ -13072,7 +13075,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="257" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A257" s="5" t="s">
         <v>651</v>
       </c>
@@ -13107,7 +13110,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="258" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A258" s="5" t="s">
         <v>652</v>
       </c>
@@ -13142,7 +13145,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="259" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A259" s="5" t="s">
         <v>654</v>
       </c>
@@ -13177,7 +13180,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="260" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A260" s="5" t="s">
         <v>671</v>
       </c>
@@ -13212,7 +13215,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="261" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A261" s="5" t="s">
         <v>672</v>
       </c>
@@ -13247,7 +13250,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="262" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A262" s="5" t="s">
         <v>673</v>
       </c>
@@ -13282,7 +13285,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="263" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A263" s="5" t="s">
         <v>674</v>
       </c>
@@ -13317,7 +13320,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="264" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A264" s="5" t="s">
         <v>675</v>
       </c>
@@ -13352,7 +13355,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="265" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A265" s="5" t="s">
         <v>676</v>
       </c>
@@ -13387,7 +13390,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="266" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A266" s="5" t="s">
         <v>677</v>
       </c>
@@ -13422,7 +13425,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="267" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A267" s="5" t="s">
         <v>678</v>
       </c>
@@ -13457,7 +13460,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="268" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A268" s="5" t="s">
         <v>679</v>
       </c>
@@ -13492,7 +13495,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="269" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A269" s="5" t="s">
         <v>737</v>
       </c>
@@ -13531,7 +13534,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="270" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A270" s="5" t="s">
         <v>777</v>
       </c>
@@ -13570,7 +13573,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="271" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A271" s="5" t="s">
         <v>714</v>
       </c>
@@ -13605,7 +13608,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="272" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A272" s="5" t="s">
         <v>729</v>
       </c>
@@ -13644,7 +13647,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="273" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A273" s="5" t="s">
         <v>723</v>
       </c>
@@ -13683,7 +13686,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="274" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A274" s="5" t="s">
         <v>724</v>
       </c>
@@ -13722,7 +13725,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="275" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A275" s="5" t="s">
         <v>725</v>
       </c>
@@ -13761,7 +13764,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="276" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A276" s="5" t="s">
         <v>726</v>
       </c>
@@ -13800,7 +13803,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="277" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A277" s="5" t="s">
         <v>730</v>
       </c>
@@ -13839,7 +13842,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="278" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A278" s="5" t="s">
         <v>775</v>
       </c>
@@ -13878,7 +13881,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="279" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A279" s="5" t="s">
         <v>776</v>
       </c>
@@ -13917,7 +13920,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="280" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>742</v>
       </c>
@@ -13956,7 +13959,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="281" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>743</v>
       </c>
@@ -13995,7 +13998,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="282" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>744</v>
       </c>
@@ -14034,7 +14037,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="283" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>745</v>
       </c>
@@ -14073,7 +14076,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="284" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>829</v>
       </c>
@@ -14109,7 +14112,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="285" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>830</v>
       </c>
@@ -14145,7 +14148,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="286" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A286" s="5" t="s">
         <v>786</v>
       </c>
@@ -14181,7 +14184,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="287" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A287" s="5" t="s">
         <v>787</v>
       </c>
@@ -14217,7 +14220,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="288" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A288" s="5" t="s">
         <v>789</v>
       </c>
@@ -14253,7 +14256,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="289" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A289" s="5" t="s">
         <v>792</v>
       </c>
@@ -14289,7 +14292,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="290" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A290" s="5" t="s">
         <v>794</v>
       </c>
@@ -14325,7 +14328,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="291" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A291" s="5" t="s">
         <v>796</v>
       </c>
@@ -14361,7 +14364,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="292" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A292" s="5" t="s">
         <v>798</v>
       </c>
@@ -14397,7 +14400,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="293" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A293" s="5" t="s">
         <v>799</v>
       </c>
@@ -14433,7 +14436,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="294" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A294" s="5" t="s">
         <v>800</v>
       </c>
@@ -14469,7 +14472,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="295" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A295" s="5" t="s">
         <v>801</v>
       </c>
@@ -14505,7 +14508,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="296" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A296" s="5" t="s">
         <v>805</v>
       </c>
@@ -14541,7 +14544,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="297" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A297" s="5" t="s">
         <v>808</v>
       </c>
@@ -14577,7 +14580,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="298" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A298" s="5" t="s">
         <v>810</v>
       </c>
@@ -14613,7 +14616,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="299" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A299" s="5" t="s">
         <v>812</v>
       </c>
@@ -14649,7 +14652,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="300" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A300" s="5" t="s">
         <v>814</v>
       </c>
@@ -14685,7 +14688,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="301" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A301" s="5" t="s">
         <v>816</v>
       </c>
@@ -14721,7 +14724,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="302" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A302" s="5" t="s">
         <v>818</v>
       </c>
@@ -14757,7 +14760,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="303" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A303" s="5" t="s">
         <v>831</v>
       </c>

</xml_diff>